<commit_message>
Add pre entrega final
</commit_message>
<xml_diff>
--- a/P0102/09_FICHAS/N2-FP-INFORME.xlsx
+++ b/P0102/09_FICHAS/N2-FP-INFORME.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28619"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\09_FICHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C83024-CCD1-4B8D-B7D7-65EF526B5F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{F6C83024-CCD1-4B8D-B7D7-65EF526B5F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B50C11E2-9C9C-4751-A977-97E5504658B5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>CODIGO DE PROYECTO</t>
   </si>
@@ -90,13 +90,56 @@
   </si>
   <si>
     <t>PALABRAS CLAVE</t>
+  </si>
+  <si>
+    <t>P0102</t>
+  </si>
+  <si>
+    <t>PR0001</t>
+  </si>
+  <si>
+    <t>Resultados Carografía Social Taller San Marcos.pptx</t>
+  </si>
+  <si>
+    <t>s3://foa-prod-comp-fenomenologico-bucket/foa_puj_curada/P0102/03_OTROS/Resultados Carograf├нa Social Taller San Marcos.pptx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ministerio de Ambiente y Desarrollo Sostenible </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es una presentación que resume y muestra cartográficamente los hallazgos de un taller de cartografía social realizado en San Marcos, en el 2024. En las diapositivas se presentan los puntos críticos que pueden ser afectados por inundaciones en siete municipios de La Mojana: Ayapel, Guaranda, Majagual, San Benito Abad, San Jacinto del Cauca, San Marcos y Sucre. </t>
+  </si>
+  <si>
+    <t>Presentación</t>
+  </si>
+  <si>
+    <t>pptx</t>
+  </si>
+  <si>
+    <t>A partir del ejercicio de cartografía social, se identificaron causas de algunas afectaciones y las propuestas para abordarlas. Algunas de las afectaciones identificadas fueron la contaminación del agua, la salud, la pérdida de cultivos, de fauna y flora, el hacinamiento y las afectaciones emocionales y psicológicas. Como causas, se identificaron la minería, la construcción de terraplén sin tener en cuenta los cauces, la pérdida de capacidad hidráulica de los cauces. Algunas de las propuestas para afrontar estas situaciones fueron: capacitaciones a las comunidades, dragado de caños y ciénagas, control de la minería, compuertas en cierres y rompimientos, entre otros. Por último, se presentan los datos históricos desde 1950 de sequías e inundaciones en La Mojana.</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>s3://foa-prod-comp-fenomenologico-bucket/foa_puj_curada/P0102/03_OTROS\20240527_135418.jpg
+s3://foa-prod-comp-fenomenologico-bucket/foa_puj_curada/P0102/03_OTROS\20240527_135736.jpg
+s3://foa-prod-comp-fenomenologico-bucket/foa_puj_curada/P0102/03_OTROS\20240527_140057.jpg
+s3://foa-prod-comp-fenomenologico-bucket/foa_puj_curada/P0102/03_OTROS\Cartograf├нa social.xlsx
+s3://foa-prod-comp-fenomenologico-bucket/foa_puj_curada/P0102/03_OTROS\Matriz consolidada.xlsx</t>
+  </si>
+  <si>
+    <t>Variable: inundaciones</t>
+  </si>
+  <si>
+    <t>Inundación, sequía, Mojana, afectaciones, minería, Ayapel, Guaranda, Majagual, San Benito Abad, San Jacinto del Cauca, San Marcos, Sucre.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,7 +176,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -182,11 +225,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -195,6 +251,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,6 +721,13 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -683,13 +748,6 @@
         <patternFill patternType="none"/>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -739,7 +797,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{071F1EEE-F40A-4A05-BF36-E5D4A7F1ECBC}" name="Tabla2" displayName="Tabla2" ref="A1:R15" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{071F1EEE-F40A-4A05-BF36-E5D4A7F1ECBC}" name="Tabla2" displayName="Tabla2" ref="A1:R15" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" headerRowBorderDxfId="19" tableBorderDxfId="20" totalsRowBorderDxfId="18">
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{0EB386ED-25C4-4E98-8607-7E1DEB7DDB25}" name="CODIGO DE PROYECTO" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{A2B4539E-FF4A-4F1D-84B8-31E807539DC0}" name="CODIGO DE PRODUCTO" dataDxfId="16"/>
@@ -1030,12 +1088,12 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="55.28515625" customWidth="1"/>
     <col min="4" max="4" width="59.5703125" customWidth="1"/>
@@ -1043,7 +1101,7 @@
     <col min="9" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="18.140625" customWidth="1"/>
     <col min="11" max="11" width="34" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" customWidth="1"/>
     <col min="13" max="13" width="20" customWidth="1"/>
     <col min="14" max="14" width="18.28515625" customWidth="1"/>
     <col min="15" max="15" width="9.7109375" customWidth="1"/>
@@ -1051,7 +1109,7 @@
     <col min="18" max="18" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1107,27 +1165,55 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+    <row r="2" spans="1:18">
+      <c r="A2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2024</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="5"/>
+      <c r="K2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1147,7 +1233,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="5"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1167,7 +1253,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="5"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1187,7 +1273,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="5"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1207,7 +1293,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="5"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1227,7 +1313,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="5"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1247,7 +1333,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="5"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1267,7 +1353,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="5"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1287,7 +1373,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="5"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1307,7 +1393,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="5"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1327,7 +1413,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1347,7 +1433,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1367,7 +1453,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1387,10 +1473,10 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18">
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="18:18">
       <c r="R17" s="1"/>
     </row>
   </sheetData>
@@ -1556,27 +1642,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02021F42-7878-49FA-AE56-8BD3BCC0EFBB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02021F42-7878-49FA-AE56-8BD3BCC0EFBB}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CD29E99-3B6E-46DF-8BF3-E73BB64F02C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3277f09b-73d6-4795-b7e6-f63d7d60cc69"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CD29E99-3B6E-46DF-8BF3-E73BB64F02C9}"/>
 </file>
</xml_diff>